<commit_message>
Merging authentication changes to master branch
</commit_message>
<xml_diff>
--- a/data/NGQ_empty_quote_data.xlsx
+++ b/data/NGQ_empty_quote_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\ngq-test-scripts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\childerr\Documents\git_projects\NGQ\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>quoteNumber</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Opportunity and Quote Info</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>apassword</t>
   </si>
 </sst>
 </file>
@@ -58,12 +70,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="00"/>
+    <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,22 +391,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="24.90625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,8 +422,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -419,6 +444,12 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the account to ngqautotester@hpe.com
</commit_message>
<xml_diff>
--- a/data/NGQ_empty_quote_data.xlsx
+++ b/data/NGQ_empty_quote_data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\NGQ\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,10 +54,10 @@
     <t>pass</t>
   </si>
   <si>
-    <t>taousautotester@hpe.com</t>
-  </si>
-  <si>
-    <t>5810ca086fd249fe54f03436d5829007179d176ceef6d120c899</t>
+    <t>ngqautotester@hpe.com</t>
+  </si>
+  <si>
+    <t>585347198c1d5b145d3de47ef43cec6ff4731f1872dbf3e75d7d</t>
   </si>
 </sst>
 </file>
@@ -394,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +461,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="mailto:taousautotester@hpe.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update account to test account
</commit_message>
<xml_diff>
--- a/data/NGQ_empty_quote_data.xlsx
+++ b/data/NGQ_empty_quote_data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\NGQ\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,10 +54,10 @@
     <t>pass</t>
   </si>
   <si>
-    <t>taousautotester@hpe.com</t>
-  </si>
-  <si>
-    <t>5810ca086fd249fe54f03436d5829007179d176ceef6d120c899</t>
+    <t>ngqautotester@hpe.com</t>
+  </si>
+  <si>
+    <t>585347198c1d5b145d3de47ef43cec6ff4731f1872dbf3e75d7d</t>
   </si>
 </sst>
 </file>
@@ -394,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +461,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="mailto:taousautotester@hpe.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the account to yu.li9@hpe.com
</commit_message>
<xml_diff>
--- a/data/NGQ_empty_quote_data.xlsx
+++ b/data/NGQ_empty_quote_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>quoteNumber</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>585347198c1d5b145d3de47ef43cec6ff4731f1872dbf3e75d7d</t>
+  </si>
+  <si>
+    <t>yu.li9@hpe.com</t>
+  </si>
+  <si>
+    <t>58c0df4d8413a6c2992ba35e7c56670f3ca3a56ed44bd79e4b5ae79ad0e5</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,14 +460,25 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the test account's password
</commit_message>
<xml_diff>
--- a/data/NGQ_empty_quote_data.xlsx
+++ b/data/NGQ_empty_quote_data.xlsx
@@ -63,7 +63,7 @@
     <t>yu.li9@hpe.com</t>
   </si>
   <si>
-    <t>58c0df4d8413a6c2992ba35e7c56670f3ca3a56ed44bd79e4b5ae79ad0e5</t>
+    <t>58c5f2460250b85bfc3954b534209943e9abe881346b292be227c8aae426</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
Update account to test account: ngqautotester@hpe.com
</commit_message>
<xml_diff>
--- a/data/NGQ_empty_quote_data.xlsx
+++ b/data/NGQ_empty_quote_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>quoteNumber</t>
   </si>
@@ -57,13 +57,7 @@
     <t>ngqautotester@hpe.com</t>
   </si>
   <si>
-    <t>585347198c1d5b145d3de47ef43cec6ff4731f1872dbf3e75d7d</t>
-  </si>
-  <si>
-    <t>yu.li9@hpe.com</t>
-  </si>
-  <si>
-    <t>58c5f2460250b85bfc3954b534209943e9abe881346b292be227c8aae426</t>
+    <t>58d22393e6aed6fe0e28a9b20e63a85e883b946af9f1ca765172</t>
   </si>
 </sst>
 </file>
@@ -395,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -406,7 +400,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,25 +454,18 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>